<commit_message>
updates e testes finais, preparação entrega
Co-Authored-By: Júlio Sá <74595961+juliofssa@users.noreply.github.com>
Co-Authored-By: Vitor Luis <74574477+Vitor-Luis-92@users.noreply.github.com>
Co-Authored-By: anibalfarraia2020 <74573559+anibalfarraia2020@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Daily Scrum 4º Sprint.xlsx
+++ b/Daily Scrum 4º Sprint.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\upskill_java1_labprg_grupo3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B702F1-FD83-491D-AE80-2CE8DE96D2BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6F9CA8-C37C-4709-93F7-D66261830FFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="22">
   <si>
     <t>1- Whats
  been done</t>
@@ -60,89 +60,6 @@
     <t>Vitor</t>
   </si>
   <si>
-    <t>aplicacao de alguns dos conceitos BD</t>
-  </si>
-  <si>
-    <t>UC2 - PLSQL</t>
-  </si>
-  <si>
-    <t>UC4, UC6 - PLSQL</t>
-  </si>
-  <si>
-    <t>UC1, UC3 - PLSQL
-UC1 - Ligação Modelo com base de dados</t>
-  </si>
-  <si>
-    <t>UC5 - PLSQL
-Inserts Gerais</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Implementação Novas Classes TDD</t>
-  </si>
-  <si>
-    <t>Implementação Novas Classes TDD</t>
-  </si>
-  <si>
-    <t>Finalização PLSQL + ligação modelo com base de dados</t>
-  </si>
-  <si>
-    <t>nenhuma</t>
-  </si>
-  <si>
-    <t>nada a realcar</t>
-  </si>
-  <si>
-    <t>Finalização PLSQL + ligação modelo com base de dados UC1/2/3</t>
-  </si>
-  <si>
-    <t>Finalização PLSQL + ligação modelo com base de dados UC4/5</t>
-  </si>
-  <si>
-    <t>Finalização PLSQL + ligação modelo com base de dados UC4/5/6</t>
-  </si>
-  <si>
-    <t>Finalização PLSQL + ligação modelo com base de dados UC1/2/3/6</t>
-  </si>
-  <si>
-    <t>UC8</t>
-  </si>
-  <si>
-    <t>UC7</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> finalizar UC7/UC8, análise/documentação</t>
-  </si>
-  <si>
-    <t>finalizar UC7/UC8</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> finalizar UC7/UC8</t>
-  </si>
-  <si>
-    <t>Correção de Testes, Documentação, Análise</t>
-  </si>
-  <si>
-    <t>Javadocs, Análise UC8</t>
-  </si>
-  <si>
-    <t>Finalizar UC9 + Ligações e Correções BD</t>
-  </si>
-  <si>
-    <t>Terminar Análise UC8 + Javadocs</t>
-  </si>
-  <si>
-    <t>Ajudar Análise UC8, Terminar Análise UC7, UC9</t>
-  </si>
-  <si>
-    <t>Finalizar UC10 + Ligações e Correções BD</t>
-  </si>
-  <si>
-    <t>Testes à aplicação e revisão de conteúdo</t>
-  </si>
-  <si>
     <t>Leitura do enunciado e Análise dos novos Ucs</t>
   </si>
   <si>
@@ -150,6 +67,42 @@
   </si>
   <si>
     <t>Implementação UC11/12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Complementação da camada DTO</t>
+  </si>
+  <si>
+    <t>Integração com BD</t>
+  </si>
+  <si>
+    <t>Desenvolvimento classes de domínio web service</t>
+  </si>
+  <si>
+    <t>Camada Controller/Service</t>
+  </si>
+  <si>
+    <t>Camada DTO/Domain</t>
+  </si>
+  <si>
+    <t>Camada Service/Domain</t>
+  </si>
+  <si>
+    <t>Camada Repositório</t>
+  </si>
+  <si>
+    <t>Finalizações e testes do webservice</t>
+  </si>
+  <si>
+    <t>Alterações no projecto para integrar novo web-service</t>
+  </si>
+  <si>
+    <t>Javadocs, Alterações no projecto para integrar novo web-service</t>
+  </si>
+  <si>
+    <t>Testes funcionais à aplicação, correção de erros</t>
+  </si>
+  <si>
+    <t>Finalização do trabalho para entrega</t>
   </si>
 </sst>
 </file>
@@ -556,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,10 +537,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -596,10 +549,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D3" s="4"/>
     </row>
@@ -608,10 +561,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D4" s="4"/>
     </row>
@@ -620,16 +573,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D5" s="4"/>
     </row>
     <row r="7" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>44244</v>
+        <v>44259</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
@@ -649,11 +602,9 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -663,43 +614,37 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D11" s="4"/>
     </row>
     <row r="13" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>44245</v>
+        <v>44260</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>0</v>
@@ -716,60 +661,52 @@
         <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D17" s="4"/>
     </row>
     <row r="20" spans="1:4" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>44246</v>
+        <v>44263</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>0</v>
@@ -781,7 +718,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>3</v>
       </c>
@@ -789,57 +726,49 @@
         <v>12</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="69.75" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="69.75" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="46.5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D24" s="4"/>
     </row>
     <row r="26" spans="1:4" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>44249</v>
+        <v>44264</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>0</v>
@@ -856,60 +785,52 @@
         <v>3</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>15</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>23</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D30" s="4"/>
     </row>
     <row r="33" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>44250</v>
+        <v>44265</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>0</v>
@@ -926,10 +847,10 @@
         <v>3</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D34" s="4"/>
     </row>
@@ -938,10 +859,10 @@
         <v>4</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D35" s="4"/>
     </row>
@@ -950,10 +871,10 @@
         <v>5</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D36" s="4"/>
     </row>
@@ -962,16 +883,16 @@
         <v>6</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D37" s="4"/>
     </row>
     <row r="39" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>44251</v>
+        <v>44266</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>0</v>
@@ -988,10 +909,10 @@
         <v>3</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D40" s="4"/>
     </row>
@@ -1000,10 +921,10 @@
         <v>4</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D41" s="4"/>
     </row>
@@ -1012,10 +933,10 @@
         <v>5</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D42" s="4"/>
     </row>
@@ -1024,16 +945,16 @@
         <v>6</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D43" s="4"/>
     </row>
     <row r="45" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>44252</v>
+        <v>44267</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>0</v>
@@ -1050,10 +971,10 @@
         <v>3</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D46" s="4"/>
     </row>
@@ -1062,10 +983,10 @@
         <v>4</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D47" s="4"/>
     </row>
@@ -1074,10 +995,10 @@
         <v>5</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D48" s="4"/>
     </row>
@@ -1086,10 +1007,10 @@
         <v>6</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D49" s="4"/>
     </row>

</xml_diff>